<commit_message>
analytics - Creates a sheet with the misclassified wallets.
</commit_message>
<xml_diff>
--- a/data/processed/wallets_misclassified.xlsx
+++ b/data/processed/wallets_misclassified.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\n29623\projetos-git\00. Courses\Mestrado - Applying graph models to money laundry detectation\repo\data\processed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F14AA1D-7C0D-4142-81E7-23959A748528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$12</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -64,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -98,41 +107,89 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1624DF81-14AD-4BAB-9FBC-D4F4F912172C}" name="Tabela1" displayName="Tabela1" ref="A1:B12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8A199E63-28F2-4868-A717-D367538699C9}" name="Resultado" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E2C16476-EBC4-4114-9231-3EBCA4EB54DA}" name="Address" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -174,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +263,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +315,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,14 +508,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,95 +529,98 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>